<commit_message>
Atualização automática de SOLEDADE.xlsx
</commit_message>
<xml_diff>
--- a/SOLEDADE.xlsx
+++ b/SOLEDADE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD1A04A6-90B2-4544-9A41-97A1F11A562D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED7EA688-FE7A-47EF-9D9D-CBEC6C70D8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1230,7 +1230,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{30208123-F4BD-4C9D-A92C-4A34E6381A87}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{B15F9858-66C0-4108-B9EE-C223D52ADFDC}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1260,10 +1260,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7968C1D4-4747-44BF-BD3C-D2ED293D35EE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6B778AF-618F-483C-B3A1-8F0E5C661707}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1301,7 +1301,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBC1C475-BBC8-4836-9BFD-42006F4304E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1A90B12-FAEB-475D-81D4-0A5FABC7FB76}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1364,7 +1364,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5ADB945F-0C67-471A-BD5A-85F1A14BD440}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBDBB8F0-0F6A-453B-9D11-13D237631EFC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1383,7 +1383,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14B09F78-D872-BA7F-C390-820D49A79769}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DCE0842-2C34-6A3D-B77F-660973034015}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1432,7 +1432,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1611855-EFAD-C88A-60D3-16BDB1BD9316}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EBB123D-11D6-34E6-0152-C26C6F1BBC91}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1451,7 +1451,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B8F6F7A-9B72-0140-3823-FEFA989DD7CF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28793D17-75C9-2CCB-9F1C-A0381ADE2CE9}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1482,7 +1482,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB83207A-7B39-8975-47DA-369420633738}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80491EF5-F381-FB8B-0473-04BD90268B6C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1513,7 +1513,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A518127-BC4B-D2AD-9400-16596B4FBF6A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C96FDFA2-8994-1D82-3592-DD5FCB872026}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1556,7 +1556,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39CC60F1-069D-4963-9931-6D684129ABE1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9F9DC27-3BE8-4655-B4C0-C86447D22C58}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1594,7 +1594,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90F2854B-43F6-459F-8015-903C393F735B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E890DEA8-498F-441B-8688-06E362BAD212}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1637,7 +1637,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B69A8C6-1EDC-4152-BF79-C6703301E3AB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F207CE6-DE7C-4C65-9821-3491796670E0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1950,7 +1950,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3286CA4F-2216-455A-BCC4-82A808C39DED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05409E9E-7195-4EED-957F-BF92EC10369B}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>